<commit_message>
Works In Apache openOffice
</commit_message>
<xml_diff>
--- a/spreadsheetFun/JavaBooks.xlsx
+++ b/spreadsheetFun/JavaBooks.xlsx
@@ -75,6 +75,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -131,6 +140,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D3">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C3=42</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>